<commit_message>
fix radial plot with a central space below zero
</commit_message>
<xml_diff>
--- a/NCSdata/BRM_GBS_NCS_2010_2017.xlsx
+++ b/NCSdata/BRM_GBS_NCS_2010_2017.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10307"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hong/Documents/GitHub/NCViewer/NCSdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{D56FD0CF-A4F0-F44D-B24C-32374204AC37}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{84DCBC9B-63F2-0B4A-AFEA-8FC4AB4E775D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="460" windowWidth="28300" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1469,7 +1469,7 @@
   <dimension ref="A1:DN95"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -18501,11 +18501,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:DN95" xr:uid="{84E247AC-5C61-5543-A5D5-4FA36E9793CC}">
-    <sortState ref="A2:DN95">
-      <sortCondition descending="1" ref="B1:B95"/>
-    </sortState>
-  </autoFilter>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>